<commit_message>
add codes to test what criteria an uncertainty parameter affects
</commit_message>
<xml_diff>
--- a/dmsan/bwaise/scores/other_tech_scores.xlsx
+++ b/dmsan/bwaise/scores/other_tech_scores.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bfca01abaf64aab7/Coding/ds/dmsan/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bfca01abaf64aab7/Coding/ds/dmsan/bwaise/scores/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="269" documentId="13_ncr:1_{2DC58649-EA64-A941-8BC7-2C09628A1C96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E611D3AE-F7DE-4047-9B70-868E2D1E7935}"/>
+  <xr:revisionPtr revIDLastSave="278" documentId="13_ncr:1_{2DC58649-EA64-A941-8BC7-2C09628A1C96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8F8B7E9D-053A-874D-B2CC-8968C0214167}"/>
   <bookViews>
-    <workbookView xWindow="-140" yWindow="500" windowWidth="34700" windowHeight="19540" xr2:uid="{672D30C3-4BC8-BB41-BA04-8F7D3B55B551}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15940" xr2:uid="{672D30C3-4BC8-BB41-BA04-8F7D3B55B551}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSummary" sheetId="25" r:id="rId1"/>
@@ -936,10 +936,10 @@
     <t>N/A (not in spreadsheet)</t>
   </si>
   <si>
-    <t>simulated in _sys_simulation.py</t>
-  </si>
-  <si>
-    <t>baseline from here, uncertainty values consistent with input parameters used in _sys_simulation.py</t>
+    <t>baseline from here, uncertainty values consistent with input parameters used in sys_simulation.py</t>
+  </si>
+  <si>
+    <t>simulated in sys_simulation.py</t>
   </si>
 </sst>
 </file>
@@ -1404,8 +1404,8 @@
   </sheetPr>
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1723,7 +1723,7 @@
         <v>150</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="H13" s="15"/>
     </row>
@@ -1747,7 +1747,7 @@
         <v>150</v>
       </c>
       <c r="G14" s="10" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="H14" s="15"/>
     </row>
@@ -1771,7 +1771,7 @@
         <v>150</v>
       </c>
       <c r="G15" s="10" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="H15" s="15"/>
     </row>
@@ -1795,7 +1795,7 @@
         <v>150</v>
       </c>
       <c r="G16" s="10" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="H16" s="15"/>
     </row>
@@ -1843,7 +1843,7 @@
         <v>204</v>
       </c>
       <c r="G18" s="11" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="H18" s="11"/>
     </row>
@@ -1867,7 +1867,7 @@
         <v>204</v>
       </c>
       <c r="G19" s="11" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="H19" s="11"/>
     </row>
@@ -1891,7 +1891,7 @@
         <v>204</v>
       </c>
       <c r="G20" s="11" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="H20" s="11"/>
     </row>
@@ -1915,7 +1915,7 @@
         <v>54</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="22" spans="1:8" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
@@ -1938,7 +1938,7 @@
         <v>59</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H22" s="8"/>
     </row>
@@ -1986,7 +1986,7 @@
         <v>70</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="25" spans="1:8" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
@@ -2033,7 +2033,7 @@
         <v>79</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="27" spans="1:8" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
new technology improvement figures
</commit_message>
<xml_diff>
--- a/dmsan/bwaise/scores/other_tech_scores.xlsx
+++ b/dmsan/bwaise/scores/other_tech_scores.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/torimorgan/Documents/GitHub/DMsan/dmsan/bwaise/scores/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bfca01abaf64aab7/Coding/ds/dmsan/bwaise/scores/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27B7228C-4025-1B46-A0A9-B6B24CB47259}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{27B7228C-4025-1B46-A0A9-B6B24CB47259}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{77FF8481-34B6-5248-B370-EB4DBB48F8AA}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1220" windowWidth="28800" windowHeight="15880" firstSheet="1" activeTab="9" xr2:uid="{672D30C3-4BC8-BB41-BA04-8F7D3B55B551}"/>
+    <workbookView xWindow="0" yWindow="1220" windowWidth="28800" windowHeight="15880" firstSheet="2" xr2:uid="{672D30C3-4BC8-BB41-BA04-8F7D3B55B551}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSummary" sheetId="25" r:id="rId1"/>
@@ -581,9 +581,6 @@
     <t>management acceptability</t>
   </si>
   <si>
-    <t>Performance Indicator</t>
-  </si>
-  <si>
     <t>Sub-Criteria</t>
   </si>
   <si>
@@ -659,9 +656,6 @@
     <t>Resource Recovery Potential</t>
   </si>
   <si>
-    <t>Net daily user cost</t>
-  </si>
-  <si>
     <t>Net Annualized Costs</t>
   </si>
   <si>
@@ -918,6 +912,12 @@
   </si>
   <si>
     <t>simulated in sys_simulation.py</t>
+  </si>
+  <si>
+    <t>Net annual user cost</t>
+  </si>
+  <si>
+    <t>Technology Indicator</t>
   </si>
 </sst>
 </file>
@@ -1382,8 +1382,8 @@
   </sheetPr>
   <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1401,37 +1401,37 @@
   <sheetData>
     <row r="1" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>88</v>
+        <v>200</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H1" s="13"/>
     </row>
     <row r="2" spans="1:8" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>6</v>
@@ -1448,13 +1448,13 @@
     </row>
     <row r="3" spans="1:8" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>6</v>
@@ -1471,13 +1471,13 @@
     </row>
     <row r="4" spans="1:8" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>6</v>
@@ -1494,13 +1494,13 @@
     </row>
     <row r="5" spans="1:8" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>6</v>
@@ -1517,13 +1517,13 @@
     </row>
     <row r="6" spans="1:8" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>6</v>
@@ -1540,13 +1540,13 @@
     </row>
     <row r="7" spans="1:8" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>34</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>6</v>
@@ -1563,13 +1563,13 @@
     </row>
     <row r="8" spans="1:8" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>6</v>
@@ -1587,13 +1587,13 @@
     </row>
     <row r="9" spans="1:8" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>6</v>
@@ -1611,13 +1611,13 @@
     </row>
     <row r="10" spans="1:8" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>6</v>
@@ -1635,22 +1635,22 @@
     </row>
     <row r="11" spans="1:8" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="D11" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="B11" s="10" t="s">
-        <v>158</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>183</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>145</v>
-      </c>
       <c r="E11" s="10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G11" s="14" t="s">
         <v>16</v>
@@ -1659,115 +1659,115 @@
     </row>
     <row r="12" spans="1:8" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>182</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="G12" s="10" t="s">
         <v>198</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>159</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>184</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>145</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>144</v>
-      </c>
-      <c r="G12" s="10" t="s">
-        <v>200</v>
       </c>
       <c r="H12" s="15"/>
     </row>
     <row r="13" spans="1:8" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="G13" s="10" t="s">
         <v>198</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>160</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>185</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>145</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="F13" s="10" t="s">
-        <v>144</v>
-      </c>
-      <c r="G13" s="10" t="s">
-        <v>200</v>
       </c>
       <c r="H13" s="15"/>
     </row>
     <row r="14" spans="1:8" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A14" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="G14" s="10" t="s">
         <v>198</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>186</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>145</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="F14" s="10" t="s">
-        <v>144</v>
-      </c>
-      <c r="G14" s="10" t="s">
-        <v>200</v>
       </c>
       <c r="H14" s="15"/>
     </row>
     <row r="15" spans="1:8" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="G15" s="10" t="s">
         <v>198</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>150</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>187</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>145</v>
-      </c>
-      <c r="E15" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="F15" s="10" t="s">
-        <v>144</v>
-      </c>
-      <c r="G15" s="10" t="s">
-        <v>200</v>
       </c>
       <c r="H15" s="15"/>
     </row>
     <row r="16" spans="1:8" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" s="10" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F16" s="10" t="s">
         <v>11</v>
@@ -1779,13 +1779,13 @@
     </row>
     <row r="17" spans="1:8" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A17" s="11" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D17" s="11" t="s">
         <v>47</v>
@@ -1794,22 +1794,22 @@
         <v>48</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="G17" s="11" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="H17" s="11"/>
     </row>
     <row r="18" spans="1:8" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" s="11" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D18" s="11" t="s">
         <v>47</v>
@@ -1818,22 +1818,22 @@
         <v>48</v>
       </c>
       <c r="F18" s="11" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="G18" s="11" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="H18" s="11"/>
     </row>
     <row r="19" spans="1:8" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" s="11" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D19" s="11" t="s">
         <v>47</v>
@@ -1842,45 +1842,45 @@
         <v>48</v>
       </c>
       <c r="F19" s="11" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="G19" s="11" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="H19" s="11"/>
     </row>
     <row r="20" spans="1:8" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>114</v>
+        <v>199</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D20" s="6" t="s">
         <v>49</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F20" s="6" t="s">
         <v>50</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="21" spans="1:8" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A21" s="8" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D21" s="8" t="s">
         <v>51</v>
@@ -1892,19 +1892,19 @@
         <v>55</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="H21" s="8"/>
     </row>
     <row r="22" spans="1:8" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A22" s="8" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D22" s="8" t="s">
         <v>51</v>
@@ -1922,42 +1922,42 @@
     </row>
     <row r="23" spans="1:8" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A23" s="8" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D23" s="8" t="s">
         <v>51</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F23" s="8" t="s">
         <v>66</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="24" spans="1:8" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A24" s="12" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D24" s="8" t="s">
         <v>51</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F24" s="8" t="s">
         <v>11</v>
@@ -1969,42 +1969,42 @@
     </row>
     <row r="25" spans="1:8" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A25" s="12" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D25" s="8" t="s">
         <v>51</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F25" s="8" t="s">
         <v>75</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="26" spans="1:8" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A26" s="12" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D26" s="8" t="s">
         <v>51</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F26" s="8" t="s">
         <v>11</v>
@@ -2018,16 +2018,16 @@
         <v>85</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D27" s="8" t="s">
         <v>51</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F27" s="8" t="s">
         <v>11</v>
@@ -2038,19 +2038,19 @@
     </row>
     <row r="28" spans="1:8" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" s="9" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D28" s="9" t="s">
         <v>51</v>
       </c>
       <c r="E28" s="9" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F28" s="9" t="s">
         <v>66</v>
@@ -2062,19 +2062,19 @@
     </row>
     <row r="29" spans="1:8" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A29" s="9" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D29" s="9" t="s">
         <v>51</v>
       </c>
       <c r="E29" s="9" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F29" s="9" t="s">
         <v>11</v>
@@ -2101,7 +2101,7 @@
   </sheetPr>
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
@@ -2109,16 +2109,16 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E1" t="s">
         <v>29</v>
@@ -2141,7 +2141,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -2167,7 +2167,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -2193,7 +2193,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -2238,16 +2238,16 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E1" t="s">
         <v>29</v>
@@ -2270,22 +2270,22 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B2" t="s">
         <v>47</v>
       </c>
       <c r="C2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -2296,22 +2296,22 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B3" t="s">
         <v>47</v>
       </c>
       <c r="C3" t="s">
+        <v>143</v>
+      </c>
+      <c r="D3" t="s">
+        <v>147</v>
+      </c>
+      <c r="E3" t="s">
         <v>145</v>
       </c>
-      <c r="D3" t="s">
-        <v>149</v>
-      </c>
-      <c r="E3" t="s">
-        <v>147</v>
-      </c>
       <c r="F3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -2322,22 +2322,22 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B4" t="s">
         <v>47</v>
       </c>
       <c r="C4" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E4" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -2366,16 +2366,16 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E1" t="s">
         <v>29</v>
@@ -2398,22 +2398,22 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B2" t="s">
         <v>47</v>
       </c>
       <c r="C2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G2">
         <v>2</v>
@@ -2424,22 +2424,22 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B3" t="s">
         <v>47</v>
       </c>
       <c r="C3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D3" t="s">
+        <v>149</v>
+      </c>
+      <c r="E3" t="s">
         <v>151</v>
       </c>
-      <c r="E3" t="s">
-        <v>153</v>
-      </c>
       <c r="F3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G3">
         <v>3</v>
@@ -2450,22 +2450,22 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B4" t="s">
         <v>47</v>
       </c>
       <c r="C4" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G4">
         <v>2</v>
@@ -2492,16 +2492,16 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E1" t="s">
         <v>29</v>
@@ -2524,7 +2524,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B2" t="s">
         <v>51</v>
@@ -2550,7 +2550,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B3" t="s">
         <v>51</v>
@@ -2582,7 +2582,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B4" t="s">
         <v>51</v>
@@ -2625,16 +2625,16 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E1" t="s">
         <v>29</v>
@@ -2657,7 +2657,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B2" t="s">
         <v>51</v>
@@ -2683,7 +2683,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B3" t="s">
         <v>51</v>
@@ -2709,7 +2709,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B4" t="s">
         <v>51</v>
@@ -2754,16 +2754,16 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E1" t="s">
         <v>29</v>
@@ -2786,7 +2786,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B2" t="s">
         <v>51</v>
@@ -2816,12 +2816,12 @@
         <v>3.3333333333333335</v>
       </c>
       <c r="J2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B3" t="s">
         <v>51</v>
@@ -2851,12 +2851,12 @@
         <v>3.3333333333333335</v>
       </c>
       <c r="J3" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B4" t="s">
         <v>51</v>
@@ -2886,7 +2886,7 @@
         <v>365</v>
       </c>
       <c r="J4" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
   </sheetData>
@@ -2911,16 +2911,16 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E1" t="s">
         <v>29</v>
@@ -2943,7 +2943,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B2" t="s">
         <v>51</v>
@@ -2969,7 +2969,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B3" t="s">
         <v>51</v>
@@ -2995,7 +2995,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B4" t="s">
         <v>51</v>
@@ -3037,16 +3037,16 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E1" t="s">
         <v>29</v>
@@ -3069,7 +3069,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B2" t="s">
         <v>51</v>
@@ -3101,7 +3101,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B3" t="s">
         <v>51</v>
@@ -3133,7 +3133,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B4" t="s">
         <v>51</v>
@@ -3181,16 +3181,16 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E1" t="s">
         <v>29</v>
@@ -3213,7 +3213,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B2" t="s">
         <v>51</v>
@@ -3239,7 +3239,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B3" t="s">
         <v>51</v>
@@ -3265,7 +3265,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B4" t="s">
         <v>51</v>
@@ -3307,16 +3307,16 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E1" t="s">
         <v>29</v>
@@ -3339,7 +3339,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B2" t="s">
         <v>51</v>
@@ -3365,7 +3365,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B3" t="s">
         <v>51</v>
@@ -3391,7 +3391,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B4" t="s">
         <v>51</v>
@@ -3438,16 +3438,16 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E1" t="s">
         <v>29</v>
@@ -3470,7 +3470,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -3496,7 +3496,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -3522,7 +3522,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -3564,16 +3564,16 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E1" t="s">
         <v>29</v>
@@ -3596,7 +3596,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B2" t="s">
         <v>51</v>
@@ -3605,10 +3605,10 @@
         <v>87</v>
       </c>
       <c r="D2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E2" t="s">
         <v>105</v>
-      </c>
-      <c r="E2" t="s">
-        <v>106</v>
       </c>
       <c r="F2" t="s">
         <v>11</v>
@@ -3622,7 +3622,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B3" t="s">
         <v>51</v>
@@ -3631,10 +3631,10 @@
         <v>87</v>
       </c>
       <c r="D3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F3" t="s">
         <v>11</v>
@@ -3648,7 +3648,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B4" t="s">
         <v>51</v>
@@ -3657,10 +3657,10 @@
         <v>87</v>
       </c>
       <c r="D4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F4" t="s">
         <v>11</v>
@@ -3690,16 +3690,16 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E1" t="s">
         <v>29</v>
@@ -3722,7 +3722,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B2" t="s">
         <v>51</v>
@@ -3731,10 +3731,10 @@
         <v>87</v>
       </c>
       <c r="D2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F2" t="s">
         <v>11</v>
@@ -3748,7 +3748,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B3" t="s">
         <v>51</v>
@@ -3757,10 +3757,10 @@
         <v>87</v>
       </c>
       <c r="D3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F3" t="s">
         <v>11</v>
@@ -3774,7 +3774,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B4" t="s">
         <v>51</v>
@@ -3783,10 +3783,10 @@
         <v>87</v>
       </c>
       <c r="D4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F4" t="s">
         <v>11</v>
@@ -3822,16 +3822,16 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E1" t="s">
         <v>29</v>
@@ -3854,7 +3854,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -3880,7 +3880,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -3906,7 +3906,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -3955,16 +3955,16 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E1" t="s">
         <v>29</v>
@@ -3987,7 +3987,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -4013,7 +4013,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -4039,7 +4039,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -4087,16 +4087,16 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E1" t="s">
         <v>29</v>
@@ -4119,7 +4119,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -4145,7 +4145,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -4171,7 +4171,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -4216,16 +4216,16 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E1" t="s">
         <v>29</v>
@@ -4248,7 +4248,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -4274,7 +4274,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -4300,7 +4300,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -4345,16 +4345,16 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E1" t="s">
         <v>29</v>
@@ -4377,7 +4377,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -4403,7 +4403,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -4429,7 +4429,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -4477,16 +4477,16 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E1" t="s">
         <v>29</v>
@@ -4509,7 +4509,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -4535,7 +4535,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -4561,7 +4561,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -4606,16 +4606,16 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E1" t="s">
         <v>29</v>
@@ -4638,7 +4638,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -4647,10 +4647,10 @@
         <v>38</v>
       </c>
       <c r="D2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F2" t="s">
         <v>11</v>
@@ -4664,7 +4664,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -4673,10 +4673,10 @@
         <v>38</v>
       </c>
       <c r="D3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="F3" t="s">
         <v>11</v>
@@ -4690,7 +4690,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -4699,10 +4699,10 @@
         <v>38</v>
       </c>
       <c r="D4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F4" t="s">
         <v>11</v>

</xml_diff>